<commit_message>
Checking for update push
</commit_message>
<xml_diff>
--- a/AIIP.xlsx
+++ b/AIIP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AIIP internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8D451C-206A-4EF0-B642-AEDB141C7456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A07CAC-C945-470C-938F-0C253251ADD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{644CA440-6242-4FA4-A9BB-86A1B4E1F082}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>No</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>All cmd in git and how to practical work</t>
+  </si>
+  <si>
+    <t>Brijesh Update</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E31F520-5F27-4A74-8191-3BDCD56E615D}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +474,7 @@
     <col min="2" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,11 +501,12 @@
       <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -525,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -548,12 +552,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -576,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -599,17 +603,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -632,9 +636,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>